<commit_message>
Validacion de importar egresados
</commit_message>
<xml_diff>
--- a/bak_formato_alumnos_excel.xlsx
+++ b/bak_formato_alumnos_excel.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
   <si>
     <t>carnet</t>
   </si>
@@ -93,6 +93,9 @@
   </si>
   <si>
     <t>Ericka@gmail.com</t>
+  </si>
+  <si>
+    <t>carrera_id</t>
   </si>
 </sst>
 </file>
@@ -435,10 +438,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -452,7 +455,7 @@
     <col min="10" max="10" width="25.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -483,8 +486,11 @@
       <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="K1" s="1" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>10</v>
       </c>
@@ -515,8 +521,11 @@
       <c r="J2" s="1" t="s">
         <v>15</v>
       </c>
+      <c r="K2" s="1">
+        <v>1</v>
+      </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>16</v>
       </c>
@@ -546,6 +555,9 @@
       </c>
       <c r="J3" s="4" t="s">
         <v>20</v>
+      </c>
+      <c r="K3" s="4">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>